<commit_message>
lr update sch/sth forms
</commit_message>
<xml_diff>
--- a/SCH-STH/Impact assessments/Liberia/lr_sch_sth_impact_202401_3_kato_katz.xlsx
+++ b/SCH-STH/Impact assessments/Liberia/lr_sch_sth_impact_202401_3_kato_katz.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\SCH-STH\Impact assessments\Liberia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2CA6606-B106-42A7-95FE-70693E953E3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F9637B-95DE-4018-8342-DD6F330FF061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="119">
   <si>
     <t>type</t>
   </si>
@@ -990,10 +990,10 @@
   <dimension ref="A1:M46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H43" sqref="H43"/>
+      <selection pane="bottomRight" activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1248,7 +1248,7 @@
       <c r="K10" s="17"/>
       <c r="L10" s="28"/>
     </row>
-    <row r="11" spans="1:13" s="31" customFormat="1" ht="31.5">
+    <row r="11" spans="1:13" s="31" customFormat="1">
       <c r="A11" s="17" t="s">
         <v>113</v>
       </c>
@@ -1260,12 +1260,8 @@
       </c>
       <c r="D11" s="18"/>
       <c r="E11" s="17"/>
-      <c r="F11" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="G11" s="18" t="s">
-        <v>75</v>
-      </c>
+      <c r="F11" s="19"/>
+      <c r="G11" s="18"/>
       <c r="H11" s="19"/>
       <c r="I11" s="17"/>
       <c r="J11" s="19" t="s">
@@ -1274,7 +1270,7 @@
       <c r="K11" s="19"/>
       <c r="L11" s="19"/>
     </row>
-    <row r="12" spans="1:13" s="31" customFormat="1" ht="47.25">
+    <row r="12" spans="1:13" s="31" customFormat="1" ht="31.5">
       <c r="A12" s="17" t="s">
         <v>13</v>
       </c>

</xml_diff>